<commit_message>
Atualizando documentações do projeto
</commit_message>
<xml_diff>
--- a/2. Análise/Cronograma do Projeto.xlsx
+++ b/2. Análise/Cronograma do Projeto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="16212"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="16215"/>
   </bookViews>
   <sheets>
     <sheet name="CronogramaDeProjeto" sheetId="11" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="término_da_tarefa" localSheetId="0">CronogramaDeProjeto!$F1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">CronogramaDeProjeto!$4:$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Crie um cronograma de projeto nesta planilha.
 Digite o título desse projeto na célula B1. 
@@ -104,12 +104,6 @@
     <t>Esta é uma linha vazia</t>
   </si>
   <si>
-    <t>Nome da empresa</t>
-  </si>
-  <si>
-    <t>Líder do projeto</t>
-  </si>
-  <si>
     <t>TAREFA</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
   <si>
     <t>Esta linha marca o final do Cronograma de projeto. NÃO insira nada nessa linha. 
 Insira novas linhas ACIMA desta linha para continuar a construção do cronograma de projeto.</t>
-  </si>
-  <si>
-    <t>Running in the world</t>
   </si>
   <si>
     <t>Agenda de corridas</t>
@@ -192,11 +183,14 @@
   <si>
     <t>Implementar a divulgação de publicações em redes sociais</t>
   </si>
+  <si>
+    <t>Running Around The World</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="9">
     <numFmt numFmtId="42" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
@@ -206,7 +200,7 @@
     <numFmt numFmtId="167" formatCode="[$-416]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="168" formatCode="d"/>
     <numFmt numFmtId="169" formatCode="d/m/yy;@"/>
-    <numFmt numFmtId="171" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="29" x14ac:knownFonts="1">
     <font>
@@ -1113,25 +1107,6 @@
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1208,67 +1183,67 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="48" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="48" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="49" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="7" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="7" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="4" fillId="45" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="170" fontId="8" fillId="46" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
@@ -1285,6 +1260,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2891,29 +2885,29 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="2.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5546875" customWidth="1"/>
-    <col min="65" max="120" width="3.44140625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.5703125" customWidth="1"/>
+    <col min="65" max="120" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2922,685 +2916,681 @@
       <c r="H1" s="2"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="56"/>
+      <c r="B2" s="39"/>
+      <c r="F2" s="49"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="52">
+      <c r="B3" s="40"/>
+      <c r="C3" s="104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="105"/>
+      <c r="E3" s="107">
         <v>43705</v>
       </c>
-      <c r="F3" s="52"/>
+      <c r="F3" s="107"/>
     </row>
-    <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="54"/>
+      <c r="C4" s="104" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="105"/>
       <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="49">
+        <v>2</v>
+      </c>
+      <c r="I4" s="101">
         <f>I5</f>
-        <v>43703</v>
-      </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="49">
+        <v>43710</v>
+      </c>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="101">
         <f>P5</f>
-        <v>43710</v>
-      </c>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="51"/>
-      <c r="W4" s="49">
+        <v>43717</v>
+      </c>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="101">
         <f>W5</f>
-        <v>43717</v>
-      </c>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="51"/>
-      <c r="AD4" s="49">
+        <v>43724</v>
+      </c>
+      <c r="X4" s="102"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="102"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="102"/>
+      <c r="AC4" s="103"/>
+      <c r="AD4" s="101">
         <f>AD5</f>
-        <v>43724</v>
-      </c>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="51"/>
-      <c r="AK4" s="49">
+        <v>43731</v>
+      </c>
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="102"/>
+      <c r="AG4" s="102"/>
+      <c r="AH4" s="102"/>
+      <c r="AI4" s="102"/>
+      <c r="AJ4" s="103"/>
+      <c r="AK4" s="101">
         <f>AK5</f>
-        <v>43731</v>
-      </c>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="50"/>
-      <c r="AN4" s="50"/>
-      <c r="AO4" s="50"/>
-      <c r="AP4" s="50"/>
-      <c r="AQ4" s="51"/>
-      <c r="AR4" s="49">
+        <v>43738</v>
+      </c>
+      <c r="AL4" s="102"/>
+      <c r="AM4" s="102"/>
+      <c r="AN4" s="102"/>
+      <c r="AO4" s="102"/>
+      <c r="AP4" s="102"/>
+      <c r="AQ4" s="103"/>
+      <c r="AR4" s="101">
         <f>AR5</f>
-        <v>43738</v>
-      </c>
-      <c r="AS4" s="50"/>
-      <c r="AT4" s="50"/>
-      <c r="AU4" s="50"/>
-      <c r="AV4" s="50"/>
-      <c r="AW4" s="50"/>
-      <c r="AX4" s="51"/>
-      <c r="AY4" s="49">
+        <v>43745</v>
+      </c>
+      <c r="AS4" s="102"/>
+      <c r="AT4" s="102"/>
+      <c r="AU4" s="102"/>
+      <c r="AV4" s="102"/>
+      <c r="AW4" s="102"/>
+      <c r="AX4" s="103"/>
+      <c r="AY4" s="101">
         <f>AY5</f>
-        <v>43745</v>
-      </c>
-      <c r="AZ4" s="50"/>
-      <c r="BA4" s="50"/>
-      <c r="BB4" s="50"/>
-      <c r="BC4" s="50"/>
-      <c r="BD4" s="50"/>
-      <c r="BE4" s="51"/>
-      <c r="BF4" s="49">
+        <v>43752</v>
+      </c>
+      <c r="AZ4" s="102"/>
+      <c r="BA4" s="102"/>
+      <c r="BB4" s="102"/>
+      <c r="BC4" s="102"/>
+      <c r="BD4" s="102"/>
+      <c r="BE4" s="103"/>
+      <c r="BF4" s="101">
         <f>BF5</f>
-        <v>43752</v>
-      </c>
-      <c r="BG4" s="50"/>
-      <c r="BH4" s="50"/>
-      <c r="BI4" s="50"/>
-      <c r="BJ4" s="50"/>
-      <c r="BK4" s="50"/>
-      <c r="BL4" s="51"/>
-      <c r="BM4" s="49">
+        <v>43759</v>
+      </c>
+      <c r="BG4" s="102"/>
+      <c r="BH4" s="102"/>
+      <c r="BI4" s="102"/>
+      <c r="BJ4" s="102"/>
+      <c r="BK4" s="102"/>
+      <c r="BL4" s="103"/>
+      <c r="BM4" s="101">
         <f>BM5</f>
-        <v>43759</v>
-      </c>
-      <c r="BN4" s="50"/>
-      <c r="BO4" s="50"/>
-      <c r="BP4" s="50"/>
-      <c r="BQ4" s="50"/>
-      <c r="BR4" s="50"/>
-      <c r="BS4" s="51"/>
-      <c r="BT4" s="49">
+        <v>43766</v>
+      </c>
+      <c r="BN4" s="102"/>
+      <c r="BO4" s="102"/>
+      <c r="BP4" s="102"/>
+      <c r="BQ4" s="102"/>
+      <c r="BR4" s="102"/>
+      <c r="BS4" s="103"/>
+      <c r="BT4" s="101">
         <f>BT5</f>
-        <v>43766</v>
-      </c>
-      <c r="BU4" s="50"/>
-      <c r="BV4" s="50"/>
-      <c r="BW4" s="50"/>
-      <c r="BX4" s="50"/>
-      <c r="BY4" s="50"/>
-      <c r="BZ4" s="51"/>
-      <c r="CA4" s="49">
+        <v>43773</v>
+      </c>
+      <c r="BU4" s="102"/>
+      <c r="BV4" s="102"/>
+      <c r="BW4" s="102"/>
+      <c r="BX4" s="102"/>
+      <c r="BY4" s="102"/>
+      <c r="BZ4" s="103"/>
+      <c r="CA4" s="101">
         <f>CA5</f>
-        <v>43773</v>
-      </c>
-      <c r="CB4" s="50"/>
-      <c r="CC4" s="50"/>
-      <c r="CD4" s="50"/>
-      <c r="CE4" s="50"/>
-      <c r="CF4" s="50"/>
-      <c r="CG4" s="51"/>
-      <c r="CH4" s="49">
+        <v>43780</v>
+      </c>
+      <c r="CB4" s="102"/>
+      <c r="CC4" s="102"/>
+      <c r="CD4" s="102"/>
+      <c r="CE4" s="102"/>
+      <c r="CF4" s="102"/>
+      <c r="CG4" s="103"/>
+      <c r="CH4" s="101">
         <f>CH5</f>
-        <v>43780</v>
-      </c>
-      <c r="CI4" s="50"/>
-      <c r="CJ4" s="50"/>
-      <c r="CK4" s="50"/>
-      <c r="CL4" s="50"/>
-      <c r="CM4" s="50"/>
-      <c r="CN4" s="51"/>
-      <c r="CO4" s="49">
+        <v>43787</v>
+      </c>
+      <c r="CI4" s="102"/>
+      <c r="CJ4" s="102"/>
+      <c r="CK4" s="102"/>
+      <c r="CL4" s="102"/>
+      <c r="CM4" s="102"/>
+      <c r="CN4" s="103"/>
+      <c r="CO4" s="101">
         <f>CO5</f>
-        <v>43787</v>
-      </c>
-      <c r="CP4" s="50"/>
-      <c r="CQ4" s="50"/>
-      <c r="CR4" s="50"/>
-      <c r="CS4" s="50"/>
-      <c r="CT4" s="50"/>
-      <c r="CU4" s="51"/>
-      <c r="CV4" s="49">
+        <v>43794</v>
+      </c>
+      <c r="CP4" s="102"/>
+      <c r="CQ4" s="102"/>
+      <c r="CR4" s="102"/>
+      <c r="CS4" s="102"/>
+      <c r="CT4" s="102"/>
+      <c r="CU4" s="103"/>
+      <c r="CV4" s="101">
         <f>CV5</f>
-        <v>43794</v>
-      </c>
-      <c r="CW4" s="50"/>
-      <c r="CX4" s="50"/>
-      <c r="CY4" s="50"/>
-      <c r="CZ4" s="50"/>
-      <c r="DA4" s="50"/>
-      <c r="DB4" s="51"/>
-      <c r="DC4" s="49">
+        <v>43801</v>
+      </c>
+      <c r="CW4" s="102"/>
+      <c r="CX4" s="102"/>
+      <c r="CY4" s="102"/>
+      <c r="CZ4" s="102"/>
+      <c r="DA4" s="102"/>
+      <c r="DB4" s="103"/>
+      <c r="DC4" s="101">
         <f>DC5</f>
-        <v>43801</v>
-      </c>
-      <c r="DD4" s="50"/>
-      <c r="DE4" s="50"/>
-      <c r="DF4" s="50"/>
-      <c r="DG4" s="50"/>
-      <c r="DH4" s="50"/>
-      <c r="DI4" s="51"/>
-      <c r="DJ4" s="49">
+        <v>43808</v>
+      </c>
+      <c r="DD4" s="102"/>
+      <c r="DE4" s="102"/>
+      <c r="DF4" s="102"/>
+      <c r="DG4" s="102"/>
+      <c r="DH4" s="102"/>
+      <c r="DI4" s="103"/>
+      <c r="DJ4" s="101">
         <f>DJ5</f>
-        <v>43808</v>
-      </c>
-      <c r="DK4" s="50"/>
-      <c r="DL4" s="50"/>
-      <c r="DM4" s="50"/>
-      <c r="DN4" s="50"/>
-      <c r="DO4" s="50"/>
-      <c r="DP4" s="51"/>
+        <v>43815</v>
+      </c>
+      <c r="DK4" s="102"/>
+      <c r="DL4" s="102"/>
+      <c r="DM4" s="102"/>
+      <c r="DN4" s="102"/>
+      <c r="DO4" s="102"/>
+      <c r="DP4" s="103"/>
     </row>
-    <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:120" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
       <c r="I5" s="43">
         <f>Início_do_projeto-WEEKDAY(Início_do_projeto,1)+2+7*(Semana_de_exibição-1)</f>
-        <v>43703</v>
+        <v>43710</v>
       </c>
       <c r="J5" s="44">
         <f>I5+1</f>
-        <v>43704</v>
+        <v>43711</v>
       </c>
       <c r="K5" s="44">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>43705</v>
+        <v>43712</v>
       </c>
       <c r="L5" s="44">
         <f t="shared" si="0"/>
-        <v>43706</v>
+        <v>43713</v>
       </c>
       <c r="M5" s="44">
         <f t="shared" si="0"/>
-        <v>43707</v>
+        <v>43714</v>
       </c>
       <c r="N5" s="44">
         <f t="shared" si="0"/>
-        <v>43708</v>
+        <v>43715</v>
       </c>
       <c r="O5" s="45">
         <f t="shared" si="0"/>
-        <v>43709</v>
+        <v>43716</v>
       </c>
       <c r="P5" s="43">
         <f>O5+1</f>
-        <v>43710</v>
+        <v>43717</v>
       </c>
       <c r="Q5" s="44">
         <f>P5+1</f>
-        <v>43711</v>
+        <v>43718</v>
       </c>
       <c r="R5" s="44">
         <f t="shared" si="0"/>
-        <v>43712</v>
+        <v>43719</v>
       </c>
       <c r="S5" s="44">
         <f t="shared" si="0"/>
-        <v>43713</v>
+        <v>43720</v>
       </c>
       <c r="T5" s="44">
         <f t="shared" si="0"/>
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="U5" s="44">
         <f t="shared" si="0"/>
-        <v>43715</v>
+        <v>43722</v>
       </c>
       <c r="V5" s="45">
         <f t="shared" si="0"/>
-        <v>43716</v>
+        <v>43723</v>
       </c>
       <c r="W5" s="43">
         <f>V5+1</f>
-        <v>43717</v>
+        <v>43724</v>
       </c>
       <c r="X5" s="44">
         <f>W5+1</f>
-        <v>43718</v>
+        <v>43725</v>
       </c>
       <c r="Y5" s="44">
         <f t="shared" si="0"/>
-        <v>43719</v>
+        <v>43726</v>
       </c>
       <c r="Z5" s="44">
         <f t="shared" si="0"/>
-        <v>43720</v>
+        <v>43727</v>
       </c>
       <c r="AA5" s="44">
         <f t="shared" si="0"/>
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="AB5" s="44">
         <f t="shared" si="0"/>
-        <v>43722</v>
+        <v>43729</v>
       </c>
       <c r="AC5" s="45">
         <f t="shared" si="0"/>
-        <v>43723</v>
+        <v>43730</v>
       </c>
       <c r="AD5" s="43">
         <f>AC5+1</f>
-        <v>43724</v>
+        <v>43731</v>
       </c>
       <c r="AE5" s="44">
         <f>AD5+1</f>
-        <v>43725</v>
+        <v>43732</v>
       </c>
       <c r="AF5" s="44">
         <f t="shared" si="0"/>
-        <v>43726</v>
+        <v>43733</v>
       </c>
       <c r="AG5" s="44">
         <f t="shared" si="0"/>
-        <v>43727</v>
+        <v>43734</v>
       </c>
       <c r="AH5" s="44">
         <f t="shared" si="0"/>
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="AI5" s="44">
         <f t="shared" si="0"/>
-        <v>43729</v>
+        <v>43736</v>
       </c>
       <c r="AJ5" s="45">
         <f t="shared" si="0"/>
-        <v>43730</v>
+        <v>43737</v>
       </c>
       <c r="AK5" s="43">
         <f>AJ5+1</f>
-        <v>43731</v>
+        <v>43738</v>
       </c>
       <c r="AL5" s="44">
         <f>AK5+1</f>
-        <v>43732</v>
+        <v>43739</v>
       </c>
       <c r="AM5" s="44">
         <f t="shared" si="0"/>
-        <v>43733</v>
+        <v>43740</v>
       </c>
       <c r="AN5" s="44">
         <f t="shared" si="0"/>
-        <v>43734</v>
+        <v>43741</v>
       </c>
       <c r="AO5" s="44">
         <f t="shared" si="0"/>
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="AP5" s="44">
         <f t="shared" si="0"/>
-        <v>43736</v>
+        <v>43743</v>
       </c>
       <c r="AQ5" s="45">
         <f t="shared" si="0"/>
-        <v>43737</v>
+        <v>43744</v>
       </c>
       <c r="AR5" s="43">
         <f>AQ5+1</f>
-        <v>43738</v>
+        <v>43745</v>
       </c>
       <c r="AS5" s="44">
         <f>AR5+1</f>
-        <v>43739</v>
+        <v>43746</v>
       </c>
       <c r="AT5" s="44">
         <f t="shared" si="0"/>
-        <v>43740</v>
+        <v>43747</v>
       </c>
       <c r="AU5" s="44">
         <f t="shared" si="0"/>
-        <v>43741</v>
+        <v>43748</v>
       </c>
       <c r="AV5" s="44">
         <f t="shared" si="0"/>
-        <v>43742</v>
+        <v>43749</v>
       </c>
       <c r="AW5" s="44">
         <f t="shared" si="0"/>
-        <v>43743</v>
+        <v>43750</v>
       </c>
       <c r="AX5" s="45">
         <f t="shared" si="0"/>
-        <v>43744</v>
+        <v>43751</v>
       </c>
       <c r="AY5" s="43">
         <f>AX5+1</f>
-        <v>43745</v>
+        <v>43752</v>
       </c>
       <c r="AZ5" s="44">
         <f>AY5+1</f>
-        <v>43746</v>
+        <v>43753</v>
       </c>
       <c r="BA5" s="44">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>43747</v>
+        <v>43754</v>
       </c>
       <c r="BB5" s="44">
         <f t="shared" si="1"/>
-        <v>43748</v>
+        <v>43755</v>
       </c>
       <c r="BC5" s="44">
         <f t="shared" si="1"/>
-        <v>43749</v>
+        <v>43756</v>
       </c>
       <c r="BD5" s="44">
         <f t="shared" si="1"/>
-        <v>43750</v>
+        <v>43757</v>
       </c>
       <c r="BE5" s="45">
         <f t="shared" si="1"/>
-        <v>43751</v>
+        <v>43758</v>
       </c>
       <c r="BF5" s="43">
         <f>BE5+1</f>
-        <v>43752</v>
+        <v>43759</v>
       </c>
       <c r="BG5" s="44">
         <f>BF5+1</f>
-        <v>43753</v>
+        <v>43760</v>
       </c>
       <c r="BH5" s="44">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>43754</v>
+        <v>43761</v>
       </c>
       <c r="BI5" s="44">
         <f t="shared" si="2"/>
-        <v>43755</v>
+        <v>43762</v>
       </c>
       <c r="BJ5" s="44">
         <f t="shared" si="2"/>
-        <v>43756</v>
+        <v>43763</v>
       </c>
       <c r="BK5" s="44">
         <f t="shared" si="2"/>
-        <v>43757</v>
+        <v>43764</v>
       </c>
       <c r="BL5" s="45">
         <f t="shared" si="2"/>
-        <v>43758</v>
+        <v>43765</v>
       </c>
       <c r="BM5" s="43">
         <f>BL5+1</f>
-        <v>43759</v>
+        <v>43766</v>
       </c>
       <c r="BN5" s="44">
         <f>BM5+1</f>
-        <v>43760</v>
+        <v>43767</v>
       </c>
       <c r="BO5" s="44">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
-        <v>43761</v>
+        <v>43768</v>
       </c>
       <c r="BP5" s="44">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
-        <v>43762</v>
+        <v>43769</v>
       </c>
       <c r="BQ5" s="44">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
-        <v>43763</v>
+        <v>43770</v>
       </c>
       <c r="BR5" s="44">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
-        <v>43764</v>
+        <v>43771</v>
       </c>
       <c r="BS5" s="45">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
-        <v>43765</v>
+        <v>43772</v>
       </c>
       <c r="BT5" s="43">
         <f>BS5+1</f>
-        <v>43766</v>
+        <v>43773</v>
       </c>
       <c r="BU5" s="44">
         <f>BT5+1</f>
-        <v>43767</v>
+        <v>43774</v>
       </c>
       <c r="BV5" s="44">
         <f t="shared" ref="BV5" si="8">BU5+1</f>
-        <v>43768</v>
+        <v>43775</v>
       </c>
       <c r="BW5" s="44">
         <f t="shared" ref="BW5" si="9">BV5+1</f>
-        <v>43769</v>
+        <v>43776</v>
       </c>
       <c r="BX5" s="44">
         <f t="shared" ref="BX5" si="10">BW5+1</f>
-        <v>43770</v>
+        <v>43777</v>
       </c>
       <c r="BY5" s="44">
         <f t="shared" ref="BY5" si="11">BX5+1</f>
-        <v>43771</v>
+        <v>43778</v>
       </c>
       <c r="BZ5" s="45">
         <f t="shared" ref="BZ5" si="12">BY5+1</f>
-        <v>43772</v>
+        <v>43779</v>
       </c>
       <c r="CA5" s="43">
         <f>BZ5+1</f>
-        <v>43773</v>
+        <v>43780</v>
       </c>
       <c r="CB5" s="44">
         <f>CA5+1</f>
-        <v>43774</v>
+        <v>43781</v>
       </c>
       <c r="CC5" s="44">
         <f t="shared" ref="CC5" si="13">CB5+1</f>
-        <v>43775</v>
+        <v>43782</v>
       </c>
       <c r="CD5" s="44">
         <f t="shared" ref="CD5" si="14">CC5+1</f>
-        <v>43776</v>
+        <v>43783</v>
       </c>
       <c r="CE5" s="44">
         <f t="shared" ref="CE5" si="15">CD5+1</f>
-        <v>43777</v>
+        <v>43784</v>
       </c>
       <c r="CF5" s="44">
         <f t="shared" ref="CF5" si="16">CE5+1</f>
-        <v>43778</v>
+        <v>43785</v>
       </c>
       <c r="CG5" s="45">
         <f t="shared" ref="CG5" si="17">CF5+1</f>
-        <v>43779</v>
+        <v>43786</v>
       </c>
       <c r="CH5" s="43">
         <f>CG5+1</f>
-        <v>43780</v>
+        <v>43787</v>
       </c>
       <c r="CI5" s="44">
         <f>CH5+1</f>
-        <v>43781</v>
+        <v>43788</v>
       </c>
       <c r="CJ5" s="44">
         <f t="shared" ref="CJ5" si="18">CI5+1</f>
-        <v>43782</v>
+        <v>43789</v>
       </c>
       <c r="CK5" s="44">
         <f t="shared" ref="CK5" si="19">CJ5+1</f>
-        <v>43783</v>
+        <v>43790</v>
       </c>
       <c r="CL5" s="44">
         <f t="shared" ref="CL5" si="20">CK5+1</f>
-        <v>43784</v>
+        <v>43791</v>
       </c>
       <c r="CM5" s="44">
         <f t="shared" ref="CM5" si="21">CL5+1</f>
-        <v>43785</v>
+        <v>43792</v>
       </c>
       <c r="CN5" s="45">
         <f t="shared" ref="CN5" si="22">CM5+1</f>
-        <v>43786</v>
+        <v>43793</v>
       </c>
       <c r="CO5" s="43">
         <f>CN5+1</f>
-        <v>43787</v>
+        <v>43794</v>
       </c>
       <c r="CP5" s="44">
         <f>CO5+1</f>
-        <v>43788</v>
+        <v>43795</v>
       </c>
       <c r="CQ5" s="44">
         <f t="shared" ref="CQ5" si="23">CP5+1</f>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="CR5" s="44">
         <f t="shared" ref="CR5" si="24">CQ5+1</f>
-        <v>43790</v>
+        <v>43797</v>
       </c>
       <c r="CS5" s="44">
         <f t="shared" ref="CS5" si="25">CR5+1</f>
-        <v>43791</v>
+        <v>43798</v>
       </c>
       <c r="CT5" s="44">
         <f t="shared" ref="CT5" si="26">CS5+1</f>
-        <v>43792</v>
+        <v>43799</v>
       </c>
       <c r="CU5" s="45">
         <f t="shared" ref="CU5" si="27">CT5+1</f>
-        <v>43793</v>
+        <v>43800</v>
       </c>
       <c r="CV5" s="43">
         <f>CU5+1</f>
-        <v>43794</v>
+        <v>43801</v>
       </c>
       <c r="CW5" s="44">
         <f>CV5+1</f>
-        <v>43795</v>
+        <v>43802</v>
       </c>
       <c r="CX5" s="44">
         <f t="shared" ref="CX5" si="28">CW5+1</f>
-        <v>43796</v>
+        <v>43803</v>
       </c>
       <c r="CY5" s="44">
         <f t="shared" ref="CY5" si="29">CX5+1</f>
-        <v>43797</v>
+        <v>43804</v>
       </c>
       <c r="CZ5" s="44">
         <f t="shared" ref="CZ5" si="30">CY5+1</f>
-        <v>43798</v>
+        <v>43805</v>
       </c>
       <c r="DA5" s="44">
         <f t="shared" ref="DA5" si="31">CZ5+1</f>
-        <v>43799</v>
+        <v>43806</v>
       </c>
       <c r="DB5" s="45">
         <f t="shared" ref="DB5" si="32">DA5+1</f>
-        <v>43800</v>
+        <v>43807</v>
       </c>
       <c r="DC5" s="43">
         <f>DB5+1</f>
-        <v>43801</v>
+        <v>43808</v>
       </c>
       <c r="DD5" s="44">
         <f>DC5+1</f>
-        <v>43802</v>
+        <v>43809</v>
       </c>
       <c r="DE5" s="44">
         <f t="shared" ref="DE5" si="33">DD5+1</f>
-        <v>43803</v>
+        <v>43810</v>
       </c>
       <c r="DF5" s="44">
         <f t="shared" ref="DF5" si="34">DE5+1</f>
-        <v>43804</v>
+        <v>43811</v>
       </c>
       <c r="DG5" s="44">
         <f t="shared" ref="DG5" si="35">DF5+1</f>
-        <v>43805</v>
+        <v>43812</v>
       </c>
       <c r="DH5" s="44">
         <f t="shared" ref="DH5" si="36">DG5+1</f>
-        <v>43806</v>
+        <v>43813</v>
       </c>
       <c r="DI5" s="45">
         <f t="shared" ref="DI5" si="37">DH5+1</f>
-        <v>43807</v>
+        <v>43814</v>
       </c>
       <c r="DJ5" s="43">
         <f>DI5+1</f>
-        <v>43808</v>
+        <v>43815</v>
       </c>
       <c r="DK5" s="44">
         <f>DJ5+1</f>
-        <v>43809</v>
+        <v>43816</v>
       </c>
       <c r="DL5" s="44">
         <f t="shared" ref="DL5" si="38">DK5+1</f>
-        <v>43810</v>
+        <v>43817</v>
       </c>
       <c r="DM5" s="44">
         <f t="shared" ref="DM5" si="39">DL5+1</f>
-        <v>43811</v>
+        <v>43818</v>
       </c>
       <c r="DN5" s="44">
         <f t="shared" ref="DN5" si="40">DM5+1</f>
-        <v>43812</v>
+        <v>43819</v>
       </c>
       <c r="DO5" s="44">
         <f t="shared" ref="DO5" si="41">DN5+1</f>
-        <v>43813</v>
+        <v>43820</v>
       </c>
       <c r="DP5" s="45">
         <f t="shared" ref="DP5" si="42">DO5+1</f>
-        <v>43814</v>
+        <v>43821</v>
       </c>
     </row>
-    <row r="6" spans="1:120" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:120" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I6" s="10" t="str">
         <f t="shared" ref="I6" si="43">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -4051,7 +4041,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:120" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:120" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>6</v>
       </c>
@@ -4174,17 +4164,17 @@
       <c r="DO7" s="30"/>
       <c r="DP7" s="30"/>
     </row>
-    <row r="8" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="75"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="68"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="str">
         <f t="shared" si="47"/>
@@ -4303,23 +4293,23 @@
       <c r="DO8" s="30"/>
       <c r="DP8" s="30"/>
     </row>
-    <row r="9" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>32</v>
+      <c r="B9" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="17">
         <v>0</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="78">
         <v>43712</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="78">
         <v>43718</v>
       </c>
       <c r="G9" s="14"/>
@@ -4440,17 +4430,17 @@
       <c r="DO9" s="30"/>
       <c r="DP9" s="30"/>
     </row>
-    <row r="10" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="76"/>
+        <v>24</v>
+      </c>
+      <c r="C10" s="69"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="87"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14" t="str">
         <f t="shared" si="47"/>
@@ -4569,21 +4559,21 @@
       <c r="DO10" s="30"/>
       <c r="DP10" s="30"/>
     </row>
-    <row r="11" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34"/>
-      <c r="B11" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>33</v>
+      <c r="B11" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>30</v>
       </c>
       <c r="D11" s="20">
         <v>0</v>
       </c>
-      <c r="E11" s="88">
+      <c r="E11" s="81">
         <v>43712</v>
       </c>
-      <c r="F11" s="88">
+      <c r="F11" s="81">
         <v>43718</v>
       </c>
       <c r="G11" s="14"/>
@@ -4704,17 +4694,17 @@
       <c r="DO11" s="30"/>
       <c r="DP11" s="30"/>
     </row>
-    <row r="12" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="77"/>
+        <v>22</v>
+      </c>
+      <c r="C12" s="70"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="89"/>
-      <c r="F12" s="90"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="str">
         <f t="shared" si="47"/>
@@ -4833,21 +4823,21 @@
       <c r="DO12" s="30"/>
       <c r="DP12" s="30"/>
     </row>
-    <row r="13" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33"/>
-      <c r="B13" s="103" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>32</v>
+      <c r="B13" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>29</v>
       </c>
       <c r="D13" s="23">
         <v>0</v>
       </c>
-      <c r="E13" s="82">
+      <c r="E13" s="75">
         <v>43719</v>
       </c>
-      <c r="F13" s="82">
+      <c r="F13" s="75">
         <v>43746</v>
       </c>
       <c r="G13" s="14"/>
@@ -4968,17 +4958,17 @@
       <c r="DO13" s="30"/>
       <c r="DP13" s="30"/>
     </row>
-    <row r="14" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="78"/>
+        <v>25</v>
+      </c>
+      <c r="C14" s="71"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="92"/>
+      <c r="E14" s="84"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="str">
         <f t="shared" si="47"/>
@@ -5097,21 +5087,21 @@
       <c r="DO14" s="30"/>
       <c r="DP14" s="30"/>
     </row>
-    <row r="15" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="33"/>
-      <c r="B15" s="104" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>33</v>
+      <c r="B15" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="64" t="s">
+        <v>30</v>
       </c>
       <c r="D15" s="26">
         <v>0</v>
       </c>
-      <c r="E15" s="93">
+      <c r="E15" s="86">
         <v>43719</v>
       </c>
-      <c r="F15" s="93">
+      <c r="F15" s="86">
         <v>43746</v>
       </c>
       <c r="G15" s="14"/>
@@ -5232,17 +5222,17 @@
       <c r="DO15" s="30"/>
       <c r="DP15" s="30"/>
     </row>
-    <row r="16" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
+      <c r="B16" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="72"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="88"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="str">
         <f t="shared" si="47"/>
@@ -5361,20 +5351,20 @@
       <c r="DO16" s="30"/>
       <c r="DP16" s="30"/>
     </row>
-    <row r="17" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="33"/>
-      <c r="B17" s="105" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="72" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="64"/>
-      <c r="E17" s="96">
+      <c r="B17" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="89">
         <f>F15+1</f>
         <v>43747</v>
       </c>
-      <c r="F17" s="96">
+      <c r="F17" s="89">
         <f>E17+27</f>
         <v>43774</v>
       </c>
@@ -5496,15 +5486,15 @@
       <c r="DO17" s="30"/>
       <c r="DP17" s="30"/>
     </row>
-    <row r="18" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
-      <c r="B18" s="65" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="98"/>
+      <c r="B18" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="91"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="str">
         <f t="shared" si="47"/>
@@ -5623,19 +5613,19 @@
       <c r="DO18" s="30"/>
       <c r="DP18" s="30"/>
     </row>
-    <row r="19" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
-      <c r="B19" s="106" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="99">
+      <c r="B19" s="99" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="60"/>
+      <c r="E19" s="92">
         <v>43747</v>
       </c>
-      <c r="F19" s="99">
+      <c r="F19" s="92">
         <v>43774</v>
       </c>
       <c r="G19" s="14"/>
@@ -5756,15 +5746,15 @@
       <c r="DO19" s="30"/>
       <c r="DP19" s="30"/>
     </row>
-    <row r="20" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="33"/>
-      <c r="B20" s="59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="101"/>
+      <c r="B20" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="74"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="94"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14" t="str">
         <f t="shared" si="47"/>
@@ -5883,20 +5873,20 @@
       <c r="DO20" s="30"/>
       <c r="DP20" s="30"/>
     </row>
-    <row r="21" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
-      <c r="B21" s="107" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="61"/>
-      <c r="E21" s="102">
+      <c r="B21" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="54"/>
+      <c r="E21" s="95">
         <f>F19+1</f>
         <v>43775</v>
       </c>
-      <c r="F21" s="102">
+      <c r="F21" s="95">
         <f>E21+27</f>
         <v>43802</v>
       </c>
@@ -6018,7 +6008,7 @@
       <c r="DO21" s="30"/>
       <c r="DP21" s="30"/>
     </row>
-    <row r="22" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="33"/>
       <c r="B22" s="42"/>
       <c r="C22" s="41"/>
@@ -6140,12 +6130,12 @@
       <c r="DO22" s="30"/>
       <c r="DP22" s="30"/>
     </row>
-    <row r="23" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:120" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="48"/>
       <c r="D23" s="28"/>
@@ -6269,18 +6259,30 @@
       <c r="DO23" s="31"/>
       <c r="DP23" s="31"/>
     </row>
-    <row r="24" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="11"/>
       <c r="F25" s="35"/>
     </row>
-    <row r="26" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:120" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="CV4:DB4"/>
     <mergeCell ref="DC4:DI4"/>
     <mergeCell ref="DJ4:DP4"/>
@@ -6289,18 +6291,6 @@
     <mergeCell ref="CA4:CG4"/>
     <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="D22:D23 D7:D15">
     <cfRule type="dataBar" priority="122">

</xml_diff>